<commit_message>
Update LCD pixel calc (version 1).xlsb.xlsx
</commit_message>
<xml_diff>
--- a/LCDs/LCD pixel calc (version 1).xlsb.xlsx
+++ b/LCDs/LCD pixel calc (version 1).xlsb.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\GitHub\CodeGeneral\LCDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3736133-B152-4871-ABDB-71CA705D9B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54900CBE-5948-465E-9188-583A6C877FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,7 +77,7 @@
     <t>Mid Start</t>
   </si>
   <si>
-    <t>gyro</t>
+    <t>aa:aa:aa</t>
   </si>
 </sst>
 </file>
@@ -114,82 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -206,10 +138,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="202020"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -467,7 +399,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +490,7 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -568,7 +500,7 @@
       </c>
       <c r="B12">
         <f>LEN(B11)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -586,7 +518,7 @@
       </c>
       <c r="B15">
         <f>B14-(B12*C3/2)</f>
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>